<commit_message>
Advanced Java syllabus is complete
Advanced Java syllabus is complete
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t>Data Abstraction.</t>
+  </si>
+  <si>
+    <t>Advanced Java</t>
+  </si>
+  <si>
+    <t>Springboot</t>
+  </si>
+  <si>
+    <t>Hibernate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Real life Project </t>
+  </si>
+  <si>
+    <t>Rest API Services,Postman</t>
   </si>
 </sst>
 </file>
@@ -183,7 +198,7 @@
       <name val="Oxygen"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,14 +263,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -268,6 +288,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +563,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D25"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -560,193 +583,234 @@
     <col min="2" max="2" width="84.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="E2" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="E4" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="E5" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="E6" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="E8" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="E9" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="E10" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1">
-      <c r="A13" s="4" t="s">
+      <c r="E12" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="E13" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="E14" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>23</v>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" customHeight="1">

</xml_diff>

<commit_message>
MySQL course is done
MySQL course is done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>Rest API Services,Postman</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>MySQL installation,DDL,DML statements</t>
+  </si>
+  <si>
+    <t>DDL and DML Statements</t>
+  </si>
+  <si>
+    <t>Stored Procedures</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Back up and Restore</t>
   </si>
 </sst>
 </file>
@@ -198,7 +216,7 @@
       <name val="Oxygen"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +253,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -263,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -291,6 +315,8 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +589,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E25"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -584,10 +610,11 @@
     <col min="3" max="3" width="42.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="39.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="11" t="s">
         <v>4</v>
@@ -601,15 +628,19 @@
       <c r="E2" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="F2" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
@@ -625,8 +656,11 @@
       <c r="E4" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="F4" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -642,8 +676,11 @@
       <c r="E5" s="14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="F5" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -659,8 +696,11 @@
       <c r="E6" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="F6" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -676,8 +716,11 @@
       <c r="E7" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="F7" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -693,8 +736,11 @@
       <c r="E8" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="F8" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
@@ -710,8 +756,11 @@
       <c r="E9" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="F9" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
@@ -727,8 +776,11 @@
       <c r="E10" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="F10" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
@@ -744,8 +796,11 @@
       <c r="E11" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="F11" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -761,8 +816,11 @@
       <c r="E12" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="F12" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
@@ -778,8 +836,11 @@
       <c r="E13" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="F13" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
@@ -795,8 +856,11 @@
       <c r="E14" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="F14" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
@@ -810,6 +874,9 @@
         <v>23</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
React JS syllabus is complete
React JS syllabus is complete
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="IT-Syllabus" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -175,6 +176,120 @@
   </si>
   <si>
     <t>Back up and Restore</t>
+  </si>
+  <si>
+    <t>// import MuiButton from './components/MuiButton';</t>
+  </si>
+  <si>
+    <t>// import MuiSelect from './components/MuiSelect';</t>
+  </si>
+  <si>
+    <t>// import MuiTextField from './components/MuiTextField';</t>
+  </si>
+  <si>
+    <t>// import MuiTypography from './components/MuiTypography';</t>
+  </si>
+  <si>
+    <t>// import MuiRadioButton from './components/MuiRadioButton';</t>
+  </si>
+  <si>
+    <t>// import MuiCheckbox from './components/MuiCheckbox';</t>
+  </si>
+  <si>
+    <t>// import MuiSwitch from './components/MuiSwitch';</t>
+  </si>
+  <si>
+    <t>// import MuiRating from './components/MuiRating';</t>
+  </si>
+  <si>
+    <t>// import MuiAutoComplete from './components/MuiAutoComplete';</t>
+  </si>
+  <si>
+    <t>// import MuiLayout from './components/MuiLayout';</t>
+  </si>
+  <si>
+    <t>// import MuiCard from './components/MuiCard';</t>
+  </si>
+  <si>
+    <t>// import MuiAccordion from './components/MuiAccordion';</t>
+  </si>
+  <si>
+    <t>// import MuiImageList from './components/MuiImageList';</t>
+  </si>
+  <si>
+    <t>import MuiNavbar from './components/MuiNavbar';</t>
+  </si>
+  <si>
+    <t>// import MuiLink from './components/MuiLink';</t>
+  </si>
+  <si>
+    <t>// import MuiBreadcrumbs from './components/MuiBreadcrumbs';</t>
+  </si>
+  <si>
+    <t>// import MuiDrawer from './components/MuiDrawer';</t>
+  </si>
+  <si>
+    <t>// import MuiSpeedDial from './components/MuiSpeedDial';</t>
+  </si>
+  <si>
+    <t>// import MuiBottomNavigation from './components/MuiBottomNavigation';</t>
+  </si>
+  <si>
+    <t>// import MuiAvatar from './components/MuiAvatar';</t>
+  </si>
+  <si>
+    <t>// import MuiBadge from './components/MuiBadge';</t>
+  </si>
+  <si>
+    <t>// import MuiList from './components/MuiList';</t>
+  </si>
+  <si>
+    <t>// import MuiChip from './MuiChip';</t>
+  </si>
+  <si>
+    <t>// import MuiResponsiveness from './components/MuiResponsiveness';</t>
+  </si>
+  <si>
+    <t>// import MuiSkeleton from './components/MuiSkeleton';</t>
+  </si>
+  <si>
+    <t>// import MuiCarousel from './components/MuiCarousel';</t>
+  </si>
+  <si>
+    <t>// import SwiperDemo from './components/SwiperDemo';</t>
+  </si>
+  <si>
+    <t>React JS</t>
+  </si>
+  <si>
+    <t>Introduction to  React JS and Material UI.</t>
+  </si>
+  <si>
+    <t>MuiTypography,MuiTextbox,MuiButton</t>
+  </si>
+  <si>
+    <t>MuiSwitch,MuiRadibutton,MuiCheckbox</t>
+  </si>
+  <si>
+    <t>MuiSelect,MuiAutocomplete</t>
+  </si>
+  <si>
+    <t>MuiRating,MuiCard,MuiLayout</t>
+  </si>
+  <si>
+    <t>MuiAccordion,MuiImageList,MuiNavbar</t>
+  </si>
+  <si>
+    <t>MuiLink,MuiBreadcrumbs,MuiDrawer</t>
+  </si>
+  <si>
+    <t>MuiSpeedDial,MuiAvatar,MuiBadge</t>
+  </si>
+  <si>
+    <t>MuiList,MuiResponsiveness,MuiSkeleton</t>
+  </si>
+  <si>
+    <t>MuiCarousel,Swiperdemo</t>
   </si>
 </sst>
 </file>
@@ -216,7 +331,7 @@
       <name val="Oxygen"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +374,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -287,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -317,6 +438,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -597,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F25"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -611,10 +734,11 @@
     <col min="4" max="4" width="51.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
+    <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="11" t="s">
         <v>4</v>
@@ -631,16 +755,20 @@
       <c r="F2" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="G2" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
@@ -659,8 +787,11 @@
       <c r="F4" s="17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="G4" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
@@ -679,8 +810,11 @@
       <c r="F5" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="G5" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -699,8 +833,11 @@
       <c r="F6" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="G6" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -719,8 +856,11 @@
       <c r="F7" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+      <c r="G7" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
@@ -739,8 +879,11 @@
       <c r="F8" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+      <c r="G8" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
@@ -759,8 +902,11 @@
       <c r="F9" s="17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+      <c r="G9" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>13</v>
       </c>
@@ -779,8 +925,11 @@
       <c r="F10" s="17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+      <c r="G10" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
@@ -799,8 +948,11 @@
       <c r="F11" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="G11" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
@@ -819,8 +971,11 @@
       <c r="F12" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+      <c r="G12" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
@@ -839,8 +994,11 @@
       <c r="F13" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
+      <c r="G13" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
@@ -859,8 +1017,11 @@
       <c r="F14" s="17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+      <c r="G14" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
@@ -877,6 +1038,9 @@
         <v>44</v>
       </c>
       <c r="F15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>44</v>
       </c>
     </row>
@@ -905,4 +1069,154 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:C30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="3:3">
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3">
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3">
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3">
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3">
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3">
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3">
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3">
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
It Syllabus is in progress
It Syllabus is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -262,12 +262,6 @@
     <t>React JS</t>
   </si>
   <si>
-    <t>Introduction to  React JS and Material UI.</t>
-  </si>
-  <si>
-    <t>MuiTypography,MuiTextbox,MuiButton</t>
-  </si>
-  <si>
     <t>MuiSwitch,MuiRadibutton,MuiCheckbox</t>
   </si>
   <si>
@@ -290,6 +284,15 @@
   </si>
   <si>
     <t>MuiCarousel,Swiperdemo</t>
+  </si>
+  <si>
+    <t>Introduction to  React JS,Functional Component and Arrow Function</t>
+  </si>
+  <si>
+    <t>Introduction to  Material UI,MuiTypography,MuiTextbox,MuiButton</t>
+  </si>
+  <si>
+    <t>React Router</t>
   </si>
 </sst>
 </file>
@@ -712,7 +715,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -720,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -734,7 +737,7 @@
     <col min="4" max="4" width="51.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -788,7 +791,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
@@ -811,7 +814,7 @@
         <v>48</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
@@ -834,7 +837,7 @@
         <v>48</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
@@ -857,7 +860,7 @@
         <v>49</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
@@ -880,7 +883,7 @@
         <v>49</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
@@ -903,7 +906,7 @@
         <v>50</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
@@ -926,7 +929,7 @@
         <v>51</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
@@ -949,7 +952,7 @@
         <v>44</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
@@ -972,7 +975,7 @@
         <v>44</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
@@ -995,7 +998,7 @@
         <v>44</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1">
@@ -1018,7 +1021,7 @@
         <v>44</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
@@ -1041,14 +1044,14 @@
         <v>44</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" customHeight="1">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" ht="15" customHeight="1">
-      <c r="B18" s="1"/>
+    <row r="20" spans="2:2" ht="15" customHeight="1">
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="2:2" ht="15" customHeight="1">
       <c r="B21" s="1"/>
@@ -1061,9 +1064,6 @@
     </row>
     <row r="24" spans="2:2" ht="15" customHeight="1">
       <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="2:2" ht="15" customHeight="1">
-      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IT-Syllabus is in progress
IT-Syllabus is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19440" windowHeight="12240" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="IT-Syllabus" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Languages" sheetId="3" r:id="rId1"/>
+    <sheet name="Database" sheetId="4" r:id="rId2"/>
+    <sheet name="MS-Office" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -176,87 +177,6 @@
   </si>
   <si>
     <t>Back up and Restore</t>
-  </si>
-  <si>
-    <t>// import MuiButton from './components/MuiButton';</t>
-  </si>
-  <si>
-    <t>// import MuiSelect from './components/MuiSelect';</t>
-  </si>
-  <si>
-    <t>// import MuiTextField from './components/MuiTextField';</t>
-  </si>
-  <si>
-    <t>// import MuiTypography from './components/MuiTypography';</t>
-  </si>
-  <si>
-    <t>// import MuiRadioButton from './components/MuiRadioButton';</t>
-  </si>
-  <si>
-    <t>// import MuiCheckbox from './components/MuiCheckbox';</t>
-  </si>
-  <si>
-    <t>// import MuiSwitch from './components/MuiSwitch';</t>
-  </si>
-  <si>
-    <t>// import MuiRating from './components/MuiRating';</t>
-  </si>
-  <si>
-    <t>// import MuiAutoComplete from './components/MuiAutoComplete';</t>
-  </si>
-  <si>
-    <t>// import MuiLayout from './components/MuiLayout';</t>
-  </si>
-  <si>
-    <t>// import MuiCard from './components/MuiCard';</t>
-  </si>
-  <si>
-    <t>// import MuiAccordion from './components/MuiAccordion';</t>
-  </si>
-  <si>
-    <t>// import MuiImageList from './components/MuiImageList';</t>
-  </si>
-  <si>
-    <t>import MuiNavbar from './components/MuiNavbar';</t>
-  </si>
-  <si>
-    <t>// import MuiLink from './components/MuiLink';</t>
-  </si>
-  <si>
-    <t>// import MuiBreadcrumbs from './components/MuiBreadcrumbs';</t>
-  </si>
-  <si>
-    <t>// import MuiDrawer from './components/MuiDrawer';</t>
-  </si>
-  <si>
-    <t>// import MuiSpeedDial from './components/MuiSpeedDial';</t>
-  </si>
-  <si>
-    <t>// import MuiBottomNavigation from './components/MuiBottomNavigation';</t>
-  </si>
-  <si>
-    <t>// import MuiAvatar from './components/MuiAvatar';</t>
-  </si>
-  <si>
-    <t>// import MuiBadge from './components/MuiBadge';</t>
-  </si>
-  <si>
-    <t>// import MuiList from './components/MuiList';</t>
-  </si>
-  <si>
-    <t>// import MuiChip from './MuiChip';</t>
-  </si>
-  <si>
-    <t>// import MuiResponsiveness from './components/MuiResponsiveness';</t>
-  </si>
-  <si>
-    <t>// import MuiSkeleton from './components/MuiSkeleton';</t>
-  </si>
-  <si>
-    <t>// import MuiCarousel from './components/MuiCarousel';</t>
-  </si>
-  <si>
-    <t>// import SwiperDemo from './components/SwiperDemo';</t>
   </si>
   <si>
     <t>React JS</t>
@@ -715,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -725,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -759,7 +679,7 @@
         <v>46</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
@@ -791,7 +711,7 @@
         <v>47</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1">
@@ -814,7 +734,7 @@
         <v>48</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
@@ -837,7 +757,7 @@
         <v>48</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
@@ -860,7 +780,7 @@
         <v>49</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
@@ -883,7 +803,7 @@
         <v>49</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1">
@@ -906,7 +826,7 @@
         <v>50</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1">
@@ -929,7 +849,7 @@
         <v>51</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
@@ -952,7 +872,7 @@
         <v>44</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1">
@@ -975,7 +895,7 @@
         <v>44</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1">
@@ -998,7 +918,7 @@
         <v>44</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1">
@@ -1021,7 +941,7 @@
         <v>44</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
@@ -1073,150 +993,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:C30"/>
+  <dimension ref="A2:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="3:3">
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3">
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3">
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3">
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3">
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3">
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3">
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3">
-      <c r="C11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3">
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3">
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3">
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3">
-      <c r="C15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3">
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
-      <c r="C23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3">
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3">
-      <c r="C25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3">
-      <c r="C26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3">
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3">
-      <c r="C28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3">
-      <c r="C29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3">
-      <c r="C30" t="s">
-        <v>78</v>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Oracle Apps Course Content added in IT Syllabus file
Oracle Apps Course Content added in IT Syllabus file
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\DocsAC\Offline\BusinessManagement\Teach_Tech@anodiam\IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD024F2B-96D2-40BB-BD56-653C11EFA960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9252" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="3" r:id="rId1"/>
     <sheet name="Database-NoSQL" sheetId="4" r:id="rId2"/>
     <sheet name="MS-Office" sheetId="5" r:id="rId3"/>
     <sheet name="Tally" sheetId="6" r:id="rId4"/>
+    <sheet name="OracleApps" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="128">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -345,13 +347,88 @@
   </si>
   <si>
     <t>https://www.collegedekho.com/courses/tally-course-syllabus-subjects</t>
+  </si>
+  <si>
+    <t>Introduction to Oracle Apps</t>
+  </si>
+  <si>
+    <t>Oracle Applications</t>
+  </si>
+  <si>
+    <t>Product Directory Structure</t>
+  </si>
+  <si>
+    <t>Data Model</t>
+  </si>
+  <si>
+    <t>Responsibilities &amp; User</t>
+  </si>
+  <si>
+    <t>New Module Development</t>
+  </si>
+  <si>
+    <t>Table Registration</t>
+  </si>
+  <si>
+    <t>FlexFields</t>
+  </si>
+  <si>
+    <t>New Form Development</t>
+  </si>
+  <si>
+    <t>Defining Calendars</t>
+  </si>
+  <si>
+    <t>WHO Columns</t>
+  </si>
+  <si>
+    <t>Non-Form Functions</t>
+  </si>
+  <si>
+    <t>Search Methods</t>
+  </si>
+  <si>
+    <t>Profiles</t>
+  </si>
+  <si>
+    <t>Customization of Forms</t>
+  </si>
+  <si>
+    <t>Concurrent Processing(CP)</t>
+  </si>
+  <si>
+    <t>Flex Field Reports</t>
+  </si>
+  <si>
+    <t>Qualifiers</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Business Components</t>
+  </si>
+  <si>
+    <t>Multi Organizations</t>
+  </si>
+  <si>
+    <t>Alerts</t>
+  </si>
+  <si>
+    <t>Discoverer</t>
+  </si>
+  <si>
+    <t>Oracle Apps Topics</t>
+  </si>
+  <si>
+    <t>Needs to verify above contents of course from Oracle Apps expert professional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +468,14 @@
       <sz val="11"/>
       <color rgb="FF202124"/>
       <name val="Oxygen"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -483,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -520,6 +605,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -800,7 +886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1150,7 +1236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1274,10 +1360,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1445,7 +1531,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1" display="https://www.udemy.com/course/microsoft-office-complete-course-all-in-one-ms-office/?gbraid=0AAAAADROdO1C_KXrwpjAtUhaf5iI38QpL&amp;utm_source=adwords&amp;utm_medium=udemyads&amp;utm_campaign=DSA_Catchall_la.EN_cc.INDIA&amp;utm_content=deal4584&amp;utm_term=_._ag_82569850245_._ad_533220805577_._kw__._de_c_._dm__._pl__._ti_dsa-392722863808_._li_1007828_._pd__._&amp;matchtype=&amp;gclid=EAIaIQobChMIr4bDt7Dv_wIVMZJmAh1kFA0iEAAYASAAEgIsTfD_BwE"/>
+    <hyperlink ref="B19" r:id="rId1" display="https://www.udemy.com/course/microsoft-office-complete-course-all-in-one-ms-office/?gbraid=0AAAAADROdO1C_KXrwpjAtUhaf5iI38QpL&amp;utm_source=adwords&amp;utm_medium=udemyads&amp;utm_campaign=DSA_Catchall_la.EN_cc.INDIA&amp;utm_content=deal4584&amp;utm_term=_._ag_82569850245_._ad_533220805577_._kw__._de_c_._dm__._pl__._ti_dsa-392722863808_._li_1007828_._pd__._&amp;matchtype=&amp;gclid=EAIaIQobChMIr4bDt7Dv_wIVMZJmAh1kFA0iEAAYASAAEgIsTfD_BwE" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
@@ -1453,11 +1539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,7 +1662,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -1585,9 +1671,227 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1"/>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABABF3A-52BB-4B4E-8BE6-C3581739C64B}">
+  <dimension ref="A2:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IT Syllabus for Java updated
IT Syllabus for Java updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6195BA99-BDDD-447A-B2E9-F326F534CFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D809053-987E-43CF-9AB2-4AD153174772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Exeption in Java</t>
   </si>
   <si>
-    <t>Collections,Lambda Expression</t>
-  </si>
-  <si>
     <t>Basic programming concepts,Arrays and programming</t>
   </si>
   <si>
@@ -437,7 +434,16 @@
     <t>Kubernetes</t>
   </si>
   <si>
-    <t>Vault by Hasi Corp</t>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>Design patterns</t>
+  </si>
+  <si>
+    <t>Revise all topics</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -579,12 +585,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -622,6 +639,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -906,7 +924,7 @@
   <dimension ref="A2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -933,13 +951,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -956,22 +974,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -982,19 +1000,19 @@
         <v>0</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,22 +1020,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,16 +1049,16 @@
         <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1048,22 +1066,22 @@
         <v>11</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1074,19 +1092,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1094,22 +1112,22 @@
         <v>13</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,16 +1141,16 @@
         <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1140,22 +1158,22 @@
         <v>15</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1166,19 +1184,19 @@
         <v>23</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>2</v>
+        <v>39</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1186,22 +1204,22 @@
         <v>17</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>3</v>
+      <c r="D14" s="27" t="s">
+        <v>133</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1215,37 +1233,34 @@
         <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="E17" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
   </sheetData>
@@ -1266,7 +1281,7 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1290,7 +1305,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1302,7 +1317,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1310,7 +1325,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1318,7 +1333,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1326,7 +1341,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1334,7 +1349,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1342,7 +1357,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1350,7 +1365,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1358,7 +1373,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1366,7 +1381,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1374,7 +1389,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1382,7 +1397,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1390,7 +1405,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1417,10 +1432,10 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1433,10 +1448,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,10 +1459,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1455,10 +1470,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1466,10 +1481,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1477,10 +1492,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1488,10 +1503,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,10 +1514,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1510,10 +1525,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1521,10 +1536,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1532,10 +1547,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1543,10 +1558,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1554,18 +1569,18 @@
         <v>18</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1593,7 +1608,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1605,7 +1620,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1613,7 +1628,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1621,7 +1636,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1629,7 +1644,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1637,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1645,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1653,7 +1668,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1661,7 +1676,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1669,7 +1684,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1677,7 +1692,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1694,18 +1709,18 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1732,7 +1747,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1740,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1748,7 +1763,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1756,7 +1771,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1764,7 +1779,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1772,7 +1787,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1780,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1788,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1796,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1804,7 +1819,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1812,7 +1827,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1820,7 +1835,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1828,7 +1843,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1836,7 +1851,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1844,7 +1859,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1852,7 +1867,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1860,7 +1875,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1868,7 +1883,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1876,7 +1891,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1884,7 +1899,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1892,7 +1907,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1900,7 +1915,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1908,7 +1923,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1916,15 +1931,15 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>

</xml_diff>

<commit_message>
Sample questions of E-Professor is saved
Sample questions of E-Professor is saved
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/IT-Syllabus.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D809053-987E-43CF-9AB2-4AD153174772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6224801-CD6B-4E54-8E03-D941C102A728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
-    <sheet name="Database-NoSQL" sheetId="4" r:id="rId3"/>
-    <sheet name="MS-Office" sheetId="5" r:id="rId4"/>
-    <sheet name="Tally" sheetId="6" r:id="rId5"/>
-    <sheet name="OracleApps" sheetId="7" r:id="rId6"/>
+    <sheet name="Database-NoSQL" sheetId="4" r:id="rId2"/>
+    <sheet name="MS-Office" sheetId="5" r:id="rId3"/>
+    <sheet name="Tally" sheetId="6" r:id="rId4"/>
+    <sheet name="OracleApps" sheetId="7" r:id="rId5"/>
+    <sheet name="ComputerDiploma" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="142">
   <si>
     <t>C operators (Operators supported by the C programming language)</t>
   </si>
@@ -431,9 +431,6 @@
     <t>Kafka Messaging System,Zoo Keeper</t>
   </si>
   <si>
-    <t>Kubernetes</t>
-  </si>
-  <si>
     <t>Threads</t>
   </si>
   <si>
@@ -444,6 +441,30 @@
   </si>
   <si>
     <t>Revise all topics</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>6 Months</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Rs 10,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly </t>
+  </si>
+  <si>
+    <t>2 Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hours </t>
+  </si>
+  <si>
+    <t>2 hours</t>
   </si>
 </sst>
 </file>
@@ -923,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1141,7 +1162,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>43</v>
@@ -1187,7 +1208,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>43</v>
@@ -1210,7 +1231,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>43</v>
@@ -1233,7 +1254,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>43</v>
@@ -1270,26 +1291,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E6E0C0-205C-4ADE-98F3-511339BDF6AD}">
-  <dimension ref="B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B15"/>
   <sheetViews>
@@ -1413,12 +1414,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:B20"/>
   <sheetViews>
@@ -1732,7 +1733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABABF3A-52BB-4B4E-8BE6-C3581739C64B}">
   <dimension ref="A2:D29"/>
   <sheetViews>
@@ -1948,4 +1949,156 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C2FCFC-DC2F-4C10-9F80-C3C02CDE75C4}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="84.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>